<commit_message>
ajustado funcoes get DataBase
</commit_message>
<xml_diff>
--- a/excel/planilhasGerada/importar-parceiros-teste.xlsx
+++ b/excel/planilhasGerada/importar-parceiros-teste.xlsx
@@ -900,53 +900,119 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Cliente</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>078.162.495-94</t>
+          <t>50.148.972/0001-04</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sr. Davi Lucca Nogueira</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>Otávio Almeida</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>morph end-to-end experiences</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>4613300</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>5338</v>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>Contribuinte</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>3730</v>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" s="6" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+        <v>2851</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>24794329</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Camila Cardoso</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>31.649.075/0001-21</t>
+        </is>
+      </c>
+      <c r="O3" s="6" t="inlineStr">
+        <is>
+          <t>visualize wireless bandwidth</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" s="6" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" s="6" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" s="6" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>COBRANCA</t>
+        </is>
+      </c>
+      <c r="U3" s="6" t="inlineStr">
+        <is>
+          <t>26735581</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Ladeira Carolina Martins</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>D20GH2B8RR</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Vila Nova Dos Milionarios</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Céu Azul</t>
+        </is>
+      </c>
+      <c r="AA3" s="6" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" t="inlineStr">
@@ -956,7 +1022,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cliente</t>
+          <t>Cliente | Transportadora</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -966,485 +1032,143 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>70342918532</t>
+          <t>62950837140</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Diego Teixeira</t>
+          <t>Vitor Gabriel da Luz</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>686</v>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>4119</v>
-      </c>
+          <t>Isento</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" s="6" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Eduardo Costa</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>19845706339</t>
+        </is>
+      </c>
+      <c r="O4" s="6" t="inlineStr">
+        <is>
+          <t>integrate B2C e-commerce</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
       <c r="S4" s="6" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" s="6" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" s="6" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>COBRANCA</t>
+        </is>
+      </c>
+      <c r="U4" s="6" t="inlineStr">
+        <is>
+          <t>19475737</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Passarela Daniela da Luz</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>9PHTVNG8KS</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Vila Independencia 3ª Seção</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Marieta 3ª Seção</t>
+        </is>
+      </c>
+      <c r="AA4" s="6" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="30" customHeight="1">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Pessoa Física</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>567.324.081-35</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Maria Eduarda Cardoso</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>9121</v>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" s="6" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" s="6" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" s="6" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" s="6" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
+      <c r="O5" s="6" t="n"/>
+      <c r="S5" s="6" t="n"/>
+      <c r="U5" s="6" t="n"/>
+      <c r="AA5" s="6" t="n"/>
     </row>
     <row r="6" ht="30" customHeight="1">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>16794285355</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Valentina da Paz</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" s="6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" s="6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" s="6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" s="6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
+      <c r="O6" s="6" t="n"/>
+      <c r="S6" s="6" t="n"/>
+      <c r="U6" s="6" t="n"/>
+      <c r="AA6" s="6" t="n"/>
     </row>
     <row r="7" ht="30" customHeight="1">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Cliente | Transportadora</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>46.187.593/0001-48</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Gabriela Cardoso</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>5634</v>
-      </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" s="6" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" s="6" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" s="6" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" s="6" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
+      <c r="O7" s="6" t="n"/>
+      <c r="S7" s="6" t="n"/>
+      <c r="U7" s="6" t="n"/>
+      <c r="AA7" s="6" t="n"/>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Transportadora</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>23.907.486/0001-41</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Sra. Ana Lívia Mendes</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" s="6" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" s="6" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" s="6" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" s="6" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
+      <c r="O8" s="6" t="n"/>
+      <c r="S8" s="6" t="n"/>
+      <c r="U8" s="6" t="n"/>
+      <c r="AA8" s="6" t="n"/>
     </row>
     <row r="9" ht="30" customHeight="1">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Transportadora</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Pessoa Física</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>729.560.843-56</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Breno da Luz</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" s="6" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" s="6" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" s="6" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" s="6" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
+      <c r="O9" s="6" t="n"/>
+      <c r="S9" s="6" t="n"/>
+      <c r="U9" s="6" t="n"/>
+      <c r="AA9" s="6" t="n"/>
     </row>
     <row r="10" ht="30" customHeight="1">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Cliente | Transportadora</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>14.350.697/0001-35</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Davi Lucas Ferreira</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>1730</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" s="6" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" s="6" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" s="6" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" s="6" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
+      <c r="O10" s="6" t="n"/>
+      <c r="S10" s="6" t="n"/>
+      <c r="U10" s="6" t="n"/>
+      <c r="AA10" s="6" t="n"/>
     </row>
     <row r="11" ht="30" customHeight="1">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>68.014.937/0001-50</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Kamilly Araújo</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>8365</v>
-      </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" s="6" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" s="6" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" s="6" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" s="6" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
+      <c r="O11" s="6" t="n"/>
+      <c r="S11" s="6" t="n"/>
+      <c r="U11" s="6" t="n"/>
+      <c r="AA11" s="6" t="n"/>
     </row>
     <row r="12" ht="30" customHeight="1">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>62.853.971/0001-31</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Maria Sophia Cavalcanti</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Não Contribuinte</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>5592</v>
-      </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" s="6" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" s="6" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" s="6" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" s="6" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
+      <c r="O12" s="6" t="n"/>
+      <c r="S12" s="6" t="n"/>
+      <c r="U12" s="6" t="n"/>
+      <c r="AA12" s="6" t="n"/>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="O13" s="6" t="n"/>

</xml_diff>